<commit_message>
sprint backlog deliverable 1
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_1_ProductBacklog_1.xlsx
+++ b/TutorGroup_Deliverable_1_ProductBacklog_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7E0CEF-F77E-594A-BB80-E523DE170EEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA53FB06-B305-6A40-90E6-C2CDC05C78D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="27640" windowHeight="18900" xr2:uid="{B19E1B03-7EFB-DF44-8F32-C033DC565042}"/>
+    <workbookView xWindow="14580" yWindow="880" windowWidth="18120" windowHeight="19360" xr2:uid="{B19E1B03-7EFB-DF44-8F32-C033DC565042}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>As a general user I would like the application to be organized effectively to increase productivity.</t>
   </si>
   <si>
-    <t>As a general user I would like the main features to be easily accessible compared to less important features, as I will be using the main features the most.</t>
-  </si>
-  <si>
     <t>As a student user I would like to be able to post listings so that I can find a tutor.</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>As a general user I would like the main features to be accessible from the home page, as I will be using the main features the most.</t>
   </si>
 </sst>
 </file>
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,6 +240,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,10 +256,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,7 +558,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,16 +593,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -616,16 +613,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -636,16 +633,16 @@
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -656,16 +653,16 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -682,10 +679,10 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -696,16 +693,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -716,16 +713,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -736,16 +733,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -756,16 +753,16 @@
         <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -776,16 +773,16 @@
         <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -802,10 +799,10 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -819,13 +816,13 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -836,16 +833,16 @@
         <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -862,30 +859,30 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
+      <c r="B16" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -902,10 +899,10 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -916,16 +913,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -936,16 +933,16 @@
         <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19">
         <v>3</v>
@@ -956,16 +953,16 @@
         <v>26</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -976,16 +973,16 @@
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -996,16 +993,16 @@
         <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -1016,16 +1013,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1042,10 +1039,10 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1056,16 +1053,16 @@
         <v>10</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1076,16 +1073,16 @@
         <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -1096,16 +1093,16 @@
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1116,16 +1113,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28">
         <v>2</v>
@@ -1136,16 +1133,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -1162,10 +1159,10 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1176,16 +1173,16 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1196,16 +1193,16 @@
         <v>18</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="5">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32">
         <v>2</v>
@@ -1216,16 +1213,16 @@
         <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1236,16 +1233,16 @@
         <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -1256,16 +1253,16 @@
         <v>19</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35">
         <v>2</v>
@@ -1276,16 +1273,16 @@
         <v>20</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1296,16 +1293,16 @@
         <v>24</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F37">
         <v>3</v>
@@ -1316,16 +1313,16 @@
         <v>27</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F38">
         <v>3</v>
@@ -1336,16 +1333,16 @@
         <v>31</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39">
         <v>1</v>

</xml_diff>

<commit_message>
sprint review 1, moved 0 documents to folder
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_1_ProductBacklog_1.xlsx
+++ b/TutorGroup_Deliverable_1_ProductBacklog_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA53FB06-B305-6A40-90E6-C2CDC05C78D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C544C-28A4-3E4F-87CE-BD1E5F88ACDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="880" windowWidth="18120" windowHeight="19360" xr2:uid="{B19E1B03-7EFB-DF44-8F32-C033DC565042}"/>
+    <workbookView xWindow="15240" yWindow="480" windowWidth="18120" windowHeight="19360" xr2:uid="{B19E1B03-7EFB-DF44-8F32-C033DC565042}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>